<commit_message>
Switched back to Catalog EF Repository
</commit_message>
<xml_diff>
--- a/Part 04/Article/part03-part04.xlsx
+++ b/Part 04/Article/part03-part04.xlsx
@@ -1,6 +1,6 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x15 xr xr6 xr10">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22527"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
@@ -8,22 +8,22 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\moliveira\Documents\GitHub\RoadToMicroservices\Part 04\Article\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:40009_{850AC1B6-6340-4ABB-BA8E-42800EF2E0A5}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5095DEE6-EF69-4243-94E3-2B589C7C6814}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="part03-part04" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'part03-part04'!$B$1:$E$58</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'part03-part04'!$B$1:$E$57</definedName>
   </definedNames>
   <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="230" uniqueCount="104">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="226" uniqueCount="103">
   <si>
     <t>Filename</t>
   </si>
@@ -245,9 +245,6 @@
   </si>
   <si>
     <t>appsettings.json</t>
-  </si>
-  <si>
-    <t>MVC.csproj</t>
   </si>
   <si>
     <t>MVC.db</t>
@@ -340,7 +337,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="18" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -1043,18 +1040,9 @@
     <xf numFmtId="0" fontId="0" fillId="34" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="35" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="35" borderId="10" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="35" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="35" borderId="12" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="35" borderId="13" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="35" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="35" borderId="15" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="35" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="35" borderId="17" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="35" borderId="18" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="34" borderId="10" xfId="0" applyFill="1" applyBorder="1"/>
@@ -1076,6 +1064,15 @@
     <xf numFmtId="0" fontId="0" fillId="33" borderId="13" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="35" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="35" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="35" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="35" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="42">
@@ -1431,11 +1428,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A2:E58"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A2:E57"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A30" workbookViewId="0">
-      <selection activeCell="C35" sqref="C35:C36"/>
+    <sheetView tabSelected="1" topLeftCell="A31" workbookViewId="0">
+      <selection activeCell="A57" sqref="A57:B57"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1449,10 +1446,10 @@
   <sheetData>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B2" s="1" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
     </row>
     <row r="3" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -1467,503 +1464,503 @@
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A4" s="16" t="s">
+      <c r="A4" s="13" t="s">
+        <v>90</v>
+      </c>
+      <c r="B4" s="14" t="s">
+        <v>18</v>
+      </c>
+      <c r="C4" s="14"/>
+      <c r="D4" s="14" t="s">
+        <v>17</v>
+      </c>
+      <c r="E4" s="15" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A5" s="16" t="s">
+        <v>90</v>
+      </c>
+      <c r="B5" s="11" t="s">
+        <v>4</v>
+      </c>
+      <c r="C5" s="11"/>
+      <c r="D5" s="11" t="s">
+        <v>49</v>
+      </c>
+      <c r="E5" s="17" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A6" s="16" t="s">
+        <v>90</v>
+      </c>
+      <c r="B6" s="11" t="s">
+        <v>40</v>
+      </c>
+      <c r="C6" s="11"/>
+      <c r="D6" s="11" t="s">
+        <v>41</v>
+      </c>
+      <c r="E6" s="17" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A7" s="16" t="s">
+        <v>90</v>
+      </c>
+      <c r="B7" s="11" t="s">
+        <v>43</v>
+      </c>
+      <c r="C7" s="11"/>
+      <c r="D7" s="11" t="s">
+        <v>41</v>
+      </c>
+      <c r="E7" s="17" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A8" s="21" t="s">
+        <v>78</v>
+      </c>
+      <c r="B8" s="22"/>
+      <c r="C8" s="22" t="s">
+        <v>4</v>
+      </c>
+      <c r="D8" s="22" t="s">
+        <v>5</v>
+      </c>
+      <c r="E8" s="23" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A9" s="13" t="s">
+        <v>89</v>
+      </c>
+      <c r="B9" s="14" t="s">
+        <v>20</v>
+      </c>
+      <c r="C9" s="14"/>
+      <c r="D9" s="14" t="s">
+        <v>17</v>
+      </c>
+      <c r="E9" s="15" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A10" s="16" t="s">
+        <v>89</v>
+      </c>
+      <c r="B10" s="11" t="s">
+        <v>31</v>
+      </c>
+      <c r="C10" s="11"/>
+      <c r="D10" s="11" t="s">
+        <v>28</v>
+      </c>
+      <c r="E10" s="17" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A11" s="16" t="s">
+        <v>89</v>
+      </c>
+      <c r="B11" s="11" t="s">
+        <v>33</v>
+      </c>
+      <c r="C11" s="11"/>
+      <c r="D11" s="11" t="s">
+        <v>28</v>
+      </c>
+      <c r="E11" s="17" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A12" s="16" t="s">
         <v>91</v>
       </c>
-      <c r="B4" s="17" t="s">
-        <v>18</v>
-      </c>
-      <c r="C4" s="17"/>
-      <c r="D4" s="17" t="s">
+      <c r="B12" s="11" t="s">
+        <v>10</v>
+      </c>
+      <c r="C12" s="11"/>
+      <c r="D12" s="11" t="s">
+        <v>3</v>
+      </c>
+      <c r="E12" s="17" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A13" s="16" t="s">
+        <v>89</v>
+      </c>
+      <c r="B13" s="11" t="s">
+        <v>34</v>
+      </c>
+      <c r="C13" s="11"/>
+      <c r="D13" s="11" t="s">
+        <v>28</v>
+      </c>
+      <c r="E13" s="17" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A14" s="16" t="s">
+        <v>89</v>
+      </c>
+      <c r="B14" s="11" t="s">
+        <v>7</v>
+      </c>
+      <c r="C14" s="11"/>
+      <c r="D14" s="11" t="s">
+        <v>49</v>
+      </c>
+      <c r="E14" s="17" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A15" s="16" t="s">
+        <v>89</v>
+      </c>
+      <c r="B15" s="11" t="s">
+        <v>44</v>
+      </c>
+      <c r="C15" s="11"/>
+      <c r="D15" s="11" t="s">
+        <v>41</v>
+      </c>
+      <c r="E15" s="17" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A16" s="16" t="s">
+        <v>89</v>
+      </c>
+      <c r="B16" s="11" t="s">
+        <v>45</v>
+      </c>
+      <c r="C16" s="11"/>
+      <c r="D16" s="11" t="s">
+        <v>41</v>
+      </c>
+      <c r="E16" s="17" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A17" s="16" t="s">
+        <v>89</v>
+      </c>
+      <c r="B17" s="11" t="s">
+        <v>46</v>
+      </c>
+      <c r="C17" s="11"/>
+      <c r="D17" s="11" t="s">
+        <v>41</v>
+      </c>
+      <c r="E17" s="17" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A18" s="16" t="s">
+        <v>89</v>
+      </c>
+      <c r="B18" s="11" t="s">
+        <v>47</v>
+      </c>
+      <c r="C18" s="11"/>
+      <c r="D18" s="11" t="s">
+        <v>41</v>
+      </c>
+      <c r="E18" s="17" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A19" s="16" t="s">
+        <v>89</v>
+      </c>
+      <c r="B19" s="11" t="s">
+        <v>75</v>
+      </c>
+      <c r="C19" s="11"/>
+      <c r="D19" s="11" t="s">
+        <v>3</v>
+      </c>
+      <c r="E19" s="17" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A20" s="21" t="s">
+        <v>79</v>
+      </c>
+      <c r="B20" s="22"/>
+      <c r="C20" s="22" t="s">
+        <v>7</v>
+      </c>
+      <c r="D20" s="22" t="s">
+        <v>5</v>
+      </c>
+      <c r="E20" s="23" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A21" s="13" t="s">
+        <v>94</v>
+      </c>
+      <c r="B21" s="14" t="s">
+        <v>21</v>
+      </c>
+      <c r="C21" s="14"/>
+      <c r="D21" s="14" t="s">
         <v>17</v>
       </c>
-      <c r="E4" s="18" t="s">
+      <c r="E21" s="15" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A5" s="19" t="s">
-        <v>91</v>
-      </c>
-      <c r="B5" s="14" t="s">
-        <v>4</v>
-      </c>
-      <c r="C5" s="14"/>
-      <c r="D5" s="14" t="s">
+    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A22" s="16" t="s">
+        <v>94</v>
+      </c>
+      <c r="B22" s="11" t="s">
+        <v>8</v>
+      </c>
+      <c r="C22" s="11"/>
+      <c r="D22" s="11" t="s">
         <v>49</v>
       </c>
-      <c r="E5" s="20" t="s">
+      <c r="E22" s="17" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A6" s="19" t="s">
-        <v>91</v>
-      </c>
-      <c r="B6" s="14" t="s">
-        <v>40</v>
-      </c>
-      <c r="C6" s="14"/>
-      <c r="D6" s="14" t="s">
-        <v>41</v>
-      </c>
-      <c r="E6" s="20" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A7" s="19" t="s">
-        <v>91</v>
-      </c>
-      <c r="B7" s="14" t="s">
-        <v>43</v>
-      </c>
-      <c r="C7" s="14"/>
-      <c r="D7" s="14" t="s">
-        <v>41</v>
-      </c>
-      <c r="E7" s="20" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="24" t="s">
-        <v>79</v>
-      </c>
-      <c r="B8" s="25"/>
-      <c r="C8" s="25" t="s">
-        <v>4</v>
-      </c>
-      <c r="D8" s="25" t="s">
+    <row r="23" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A23" s="21" t="s">
+        <v>80</v>
+      </c>
+      <c r="B23" s="22"/>
+      <c r="C23" s="22" t="s">
+        <v>8</v>
+      </c>
+      <c r="D23" s="22" t="s">
         <v>5</v>
       </c>
-      <c r="E8" s="26" t="s">
+      <c r="E23" s="23" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A9" s="16" t="s">
-        <v>90</v>
-      </c>
-      <c r="B9" s="17" t="s">
-        <v>20</v>
-      </c>
-      <c r="C9" s="17"/>
-      <c r="D9" s="17" t="s">
+    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A24" s="13" t="s">
+        <v>93</v>
+      </c>
+      <c r="B24" s="14" t="s">
+        <v>24</v>
+      </c>
+      <c r="C24" s="14"/>
+      <c r="D24" s="14" t="s">
         <v>17</v>
       </c>
-      <c r="E9" s="18" t="s">
+      <c r="E24" s="15" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A10" s="19" t="s">
-        <v>90</v>
-      </c>
-      <c r="B10" s="14" t="s">
-        <v>31</v>
-      </c>
-      <c r="C10" s="14"/>
-      <c r="D10" s="14" t="s">
+    <row r="25" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A25" s="16" t="s">
+        <v>93</v>
+      </c>
+      <c r="B25" s="11" t="s">
+        <v>39</v>
+      </c>
+      <c r="C25" s="11"/>
+      <c r="D25" s="11" t="s">
+        <v>3</v>
+      </c>
+      <c r="E25" s="17" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A26" s="16" t="s">
+        <v>95</v>
+      </c>
+      <c r="B26" s="11" t="s">
+        <v>51</v>
+      </c>
+      <c r="C26" s="11"/>
+      <c r="D26" s="11" t="s">
+        <v>49</v>
+      </c>
+      <c r="E26" s="17" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A27" s="21" t="s">
+        <v>82</v>
+      </c>
+      <c r="B27" s="22"/>
+      <c r="C27" s="22" t="s">
+        <v>13</v>
+      </c>
+      <c r="D27" s="22" t="s">
+        <v>5</v>
+      </c>
+      <c r="E27" s="23" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A28" s="13" t="s">
+        <v>92</v>
+      </c>
+      <c r="B28" s="14" t="s">
+        <v>35</v>
+      </c>
+      <c r="C28" s="14"/>
+      <c r="D28" s="14" t="s">
         <v>28</v>
       </c>
-      <c r="E10" s="20" t="s">
+      <c r="E28" s="15" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A11" s="19" t="s">
-        <v>90</v>
-      </c>
-      <c r="B11" s="14" t="s">
-        <v>33</v>
-      </c>
-      <c r="C11" s="14"/>
-      <c r="D11" s="14" t="s">
-        <v>28</v>
-      </c>
-      <c r="E11" s="20" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A12" s="19" t="s">
+    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A29" s="16" t="s">
         <v>92</v>
       </c>
-      <c r="B12" s="14" t="s">
+      <c r="B29" s="11" t="s">
+        <v>25</v>
+      </c>
+      <c r="C29" s="11"/>
+      <c r="D29" s="11" t="s">
+        <v>17</v>
+      </c>
+      <c r="E29" s="17" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A30" s="16" t="s">
+        <v>92</v>
+      </c>
+      <c r="B30" s="11" t="s">
+        <v>14</v>
+      </c>
+      <c r="C30" s="11"/>
+      <c r="D30" s="11" t="s">
+        <v>49</v>
+      </c>
+      <c r="E30" s="17" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A31" s="21" t="s">
+        <v>83</v>
+      </c>
+      <c r="B31" s="22"/>
+      <c r="C31" s="22" t="s">
+        <v>14</v>
+      </c>
+      <c r="D31" s="22" t="s">
+        <v>5</v>
+      </c>
+      <c r="E31" s="23" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A32" s="25" t="s">
+        <v>81</v>
+      </c>
+      <c r="B32" s="26"/>
+      <c r="C32" s="26" t="s">
         <v>10</v>
       </c>
-      <c r="C12" s="14"/>
-      <c r="D12" s="14" t="s">
-        <v>3</v>
-      </c>
-      <c r="E12" s="20" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A13" s="19" t="s">
-        <v>90</v>
-      </c>
-      <c r="B13" s="14" t="s">
-        <v>34</v>
-      </c>
-      <c r="C13" s="14"/>
-      <c r="D13" s="14" t="s">
-        <v>28</v>
-      </c>
-      <c r="E13" s="20" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A14" s="19" t="s">
-        <v>90</v>
-      </c>
-      <c r="B14" s="14" t="s">
-        <v>7</v>
-      </c>
-      <c r="C14" s="14"/>
-      <c r="D14" s="14" t="s">
-        <v>49</v>
-      </c>
-      <c r="E14" s="20" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A15" s="19" t="s">
-        <v>90</v>
-      </c>
-      <c r="B15" s="14" t="s">
-        <v>44</v>
-      </c>
-      <c r="C15" s="14"/>
-      <c r="D15" s="14" t="s">
-        <v>41</v>
-      </c>
-      <c r="E15" s="20" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A16" s="19" t="s">
-        <v>90</v>
-      </c>
-      <c r="B16" s="14" t="s">
-        <v>45</v>
-      </c>
-      <c r="C16" s="14"/>
-      <c r="D16" s="14" t="s">
-        <v>41</v>
-      </c>
-      <c r="E16" s="20" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A17" s="19" t="s">
-        <v>90</v>
-      </c>
-      <c r="B17" s="14" t="s">
-        <v>46</v>
-      </c>
-      <c r="C17" s="14"/>
-      <c r="D17" s="14" t="s">
-        <v>41</v>
-      </c>
-      <c r="E17" s="20" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A18" s="19" t="s">
-        <v>90</v>
-      </c>
-      <c r="B18" s="14" t="s">
-        <v>47</v>
-      </c>
-      <c r="C18" s="14"/>
-      <c r="D18" s="14" t="s">
-        <v>41</v>
-      </c>
-      <c r="E18" s="20" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A19" s="19" t="s">
-        <v>90</v>
-      </c>
-      <c r="B19" s="14" t="s">
-        <v>76</v>
-      </c>
-      <c r="C19" s="14"/>
-      <c r="D19" s="14" t="s">
-        <v>3</v>
-      </c>
-      <c r="E19" s="20" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="20" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A20" s="24" t="s">
-        <v>80</v>
-      </c>
-      <c r="B20" s="25"/>
-      <c r="C20" s="25" t="s">
-        <v>7</v>
-      </c>
-      <c r="D20" s="25" t="s">
+      <c r="D32" s="26" t="s">
+        <v>9</v>
+      </c>
+      <c r="E32" s="27" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="33" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A33" s="18" t="s">
+        <v>81</v>
+      </c>
+      <c r="B33" s="19"/>
+      <c r="C33" s="19" t="s">
+        <v>12</v>
+      </c>
+      <c r="D33" s="19" t="s">
+        <v>9</v>
+      </c>
+      <c r="E33" s="20" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A34" s="24" t="s">
+        <v>84</v>
+      </c>
+      <c r="B34" s="24"/>
+      <c r="C34" s="24" t="s">
+        <v>15</v>
+      </c>
+      <c r="D34" s="24" t="s">
         <v>5</v>
       </c>
-      <c r="E20" s="26" t="s">
+      <c r="E34" s="24" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A21" s="16" t="s">
-        <v>95</v>
-      </c>
-      <c r="B21" s="17" t="s">
-        <v>21</v>
-      </c>
-      <c r="C21" s="17"/>
-      <c r="D21" s="17" t="s">
+    <row r="35" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A35" s="12" t="s">
+        <v>85</v>
+      </c>
+      <c r="B35" s="12"/>
+      <c r="C35" s="12" t="s">
+        <v>16</v>
+      </c>
+      <c r="D35" s="12" t="s">
+        <v>5</v>
+      </c>
+      <c r="E35" s="12" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="36" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A36" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="B36" s="12"/>
+      <c r="C36" s="12" t="s">
+        <v>22</v>
+      </c>
+      <c r="D36" s="12" t="s">
         <v>17</v>
       </c>
-      <c r="E21" s="18" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A22" s="19" t="s">
-        <v>95</v>
-      </c>
-      <c r="B22" s="14" t="s">
-        <v>8</v>
-      </c>
-      <c r="C22" s="14"/>
-      <c r="D22" s="14" t="s">
-        <v>49</v>
-      </c>
-      <c r="E22" s="20" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="23" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A23" s="24" t="s">
-        <v>81</v>
-      </c>
-      <c r="B23" s="25"/>
-      <c r="C23" s="25" t="s">
-        <v>8</v>
-      </c>
-      <c r="D23" s="25" t="s">
-        <v>5</v>
-      </c>
-      <c r="E23" s="26" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A24" s="16" t="s">
-        <v>94</v>
-      </c>
-      <c r="B24" s="17" t="s">
-        <v>24</v>
-      </c>
-      <c r="C24" s="17"/>
-      <c r="D24" s="17" t="s">
-        <v>17</v>
-      </c>
-      <c r="E24" s="18" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="25" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A25" s="19" t="s">
-        <v>94</v>
-      </c>
-      <c r="B25" s="14" t="s">
-        <v>39</v>
-      </c>
-      <c r="C25" s="14"/>
-      <c r="D25" s="14" t="s">
-        <v>3</v>
-      </c>
-      <c r="E25" s="20" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A26" s="19" t="s">
-        <v>96</v>
-      </c>
-      <c r="B26" s="14" t="s">
-        <v>51</v>
-      </c>
-      <c r="C26" s="14"/>
-      <c r="D26" s="14" t="s">
-        <v>49</v>
-      </c>
-      <c r="E26" s="20" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="27" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A27" s="24" t="s">
-        <v>83</v>
-      </c>
-      <c r="B27" s="25"/>
-      <c r="C27" s="25" t="s">
-        <v>13</v>
-      </c>
-      <c r="D27" s="25" t="s">
-        <v>5</v>
-      </c>
-      <c r="E27" s="26" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A28" s="16" t="s">
-        <v>93</v>
-      </c>
-      <c r="B28" s="17" t="s">
-        <v>35</v>
-      </c>
-      <c r="C28" s="17"/>
-      <c r="D28" s="17" t="s">
-        <v>28</v>
-      </c>
-      <c r="E28" s="18" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A29" s="19" t="s">
-        <v>93</v>
-      </c>
-      <c r="B29" s="14" t="s">
-        <v>25</v>
-      </c>
-      <c r="C29" s="14"/>
-      <c r="D29" s="14" t="s">
-        <v>17</v>
-      </c>
-      <c r="E29" s="20" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A30" s="19" t="s">
-        <v>93</v>
-      </c>
-      <c r="B30" s="14" t="s">
-        <v>14</v>
-      </c>
-      <c r="C30" s="14"/>
-      <c r="D30" s="14" t="s">
-        <v>49</v>
-      </c>
-      <c r="E30" s="20" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="31" spans="1:5" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A31" s="24" t="s">
-        <v>84</v>
-      </c>
-      <c r="B31" s="25"/>
-      <c r="C31" s="25" t="s">
-        <v>14</v>
-      </c>
-      <c r="D31" s="25" t="s">
-        <v>5</v>
-      </c>
-      <c r="E31" s="26" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="32" spans="1:5" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A32" s="28" t="s">
-        <v>82</v>
-      </c>
-      <c r="B32" s="29"/>
-      <c r="C32" s="29" t="s">
-        <v>10</v>
-      </c>
-      <c r="D32" s="29" t="s">
-        <v>9</v>
-      </c>
-      <c r="E32" s="30" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="33" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A33" s="21" t="s">
-        <v>82</v>
-      </c>
-      <c r="B33" s="22"/>
-      <c r="C33" s="22" t="s">
-        <v>12</v>
-      </c>
-      <c r="D33" s="22" t="s">
-        <v>9</v>
-      </c>
-      <c r="E33" s="23" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A34" s="27" t="s">
-        <v>85</v>
-      </c>
-      <c r="B34" s="27"/>
-      <c r="C34" s="27" t="s">
-        <v>15</v>
-      </c>
-      <c r="D34" s="27" t="s">
-        <v>5</v>
-      </c>
-      <c r="E34" s="27" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="35" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A35" s="15" t="s">
-        <v>86</v>
-      </c>
-      <c r="B35" s="15"/>
-      <c r="C35" s="15" t="s">
-        <v>16</v>
-      </c>
-      <c r="D35" s="15" t="s">
-        <v>5</v>
-      </c>
-      <c r="E35" s="15" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="36" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A36" s="15" t="s">
-        <v>89</v>
-      </c>
-      <c r="B36" s="15"/>
-      <c r="C36" s="15" t="s">
-        <v>22</v>
-      </c>
-      <c r="D36" s="15" t="s">
-        <v>17</v>
-      </c>
-      <c r="E36" s="15" t="s">
+      <c r="E36" s="12" t="s">
         <v>23</v>
       </c>
     </row>
     <row r="37" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A37" s="4" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="B37" s="4" t="s">
         <v>27</v>
@@ -1980,7 +1977,7 @@
     </row>
     <row r="38" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A38" s="4" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="B38" s="4" t="s">
         <v>30</v>
@@ -1997,7 +1994,7 @@
     </row>
     <row r="39" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A39" s="4" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="B39" s="4" t="s">
         <v>36</v>
@@ -2014,7 +2011,7 @@
     </row>
     <row r="40" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A40" s="4" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="B40" s="4" t="s">
         <v>37</v>
@@ -2133,24 +2130,24 @@
       </c>
     </row>
     <row r="48" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A48" s="6" t="s">
+      <c r="A48" s="29" t="s">
         <v>65</v>
       </c>
-      <c r="B48" s="7" t="s">
+      <c r="B48" s="6" t="s">
         <v>61</v>
       </c>
-      <c r="C48" s="7" t="s">
+      <c r="C48" s="6" t="s">
         <v>61</v>
       </c>
-      <c r="D48" s="7" t="s">
+      <c r="D48" s="6" t="s">
         <v>62</v>
       </c>
-      <c r="E48" s="8" t="s">
+      <c r="E48" s="7" t="s">
         <v>29</v>
       </c>
     </row>
     <row r="49" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A49" s="9"/>
+      <c r="A49" s="30"/>
       <c r="B49" s="5" t="s">
         <v>63</v>
       </c>
@@ -2160,12 +2157,12 @@
       <c r="D49" s="5" t="s">
         <v>62</v>
       </c>
-      <c r="E49" s="10" t="s">
+      <c r="E49" s="8" t="s">
         <v>29</v>
       </c>
     </row>
     <row r="50" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A50" s="9"/>
+      <c r="A50" s="30"/>
       <c r="B50" s="5" t="s">
         <v>64</v>
       </c>
@@ -2175,28 +2172,28 @@
       <c r="D50" s="5" t="s">
         <v>62</v>
       </c>
-      <c r="E50" s="10" t="s">
+      <c r="E50" s="8" t="s">
         <v>29</v>
       </c>
     </row>
     <row r="51" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A51" s="11"/>
-      <c r="B51" s="12" t="s">
+      <c r="A51" s="31"/>
+      <c r="B51" s="9" t="s">
         <v>67</v>
       </c>
-      <c r="C51" s="12" t="s">
+      <c r="C51" s="9" t="s">
         <v>67</v>
       </c>
-      <c r="D51" s="12" t="s">
+      <c r="D51" s="9" t="s">
         <v>66</v>
       </c>
-      <c r="E51" s="13" t="s">
+      <c r="E51" s="10" t="s">
         <v>29</v>
       </c>
     </row>
     <row r="52" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A52" s="2" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="B52" s="2"/>
       <c r="C52" s="2" t="s">
@@ -2240,26 +2237,26 @@
       </c>
     </row>
     <row r="55" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A55" s="4"/>
-      <c r="B55" s="4" t="s">
+      <c r="A55" s="3" t="s">
+        <v>96</v>
+      </c>
+      <c r="B55" s="3" t="s">
         <v>74</v>
       </c>
-      <c r="C55" s="4" t="s">
-        <v>74</v>
-      </c>
-      <c r="D55" s="4" t="s">
+      <c r="C55" s="3"/>
+      <c r="D55" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="E55" s="4" t="s">
-        <v>29</v>
+      <c r="E55" s="3" t="s">
+        <v>26</v>
       </c>
     </row>
     <row r="56" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A56" s="3" t="s">
-        <v>97</v>
+        <v>99</v>
       </c>
       <c r="B56" s="3" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="C56" s="3"/>
       <c r="D56" s="3" t="s">
@@ -2269,40 +2266,25 @@
         <v>26</v>
       </c>
     </row>
-    <row r="57" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A57" s="3" t="s">
-        <v>100</v>
-      </c>
-      <c r="B57" s="3" t="s">
+    <row r="57" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A57" s="28" t="s">
+        <v>98</v>
+      </c>
+      <c r="B57" s="4" t="s">
         <v>77</v>
       </c>
-      <c r="C57" s="3"/>
-      <c r="D57" s="3" t="s">
+      <c r="C57" s="4" t="s">
+        <v>77</v>
+      </c>
+      <c r="D57" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="E57" s="3" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="58" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="A58" s="31" t="s">
-        <v>99</v>
-      </c>
-      <c r="B58" s="4" t="s">
-        <v>78</v>
-      </c>
-      <c r="C58" s="4" t="s">
-        <v>78</v>
-      </c>
-      <c r="D58" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="E58" s="4" t="s">
+      <c r="E57" s="4" t="s">
         <v>29</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="B1:E58"/>
+  <autoFilter ref="B1:E57" xr:uid="{00000000-0009-0000-0000-000000000000}"/>
   <mergeCells count="1">
     <mergeCell ref="A48:A51"/>
   </mergeCells>

</xml_diff>